<commit_message>
- Corrected draft - Added photos used for plates
</commit_message>
<xml_diff>
--- a/analysis/data/supplementary_data/sample_macroscopicTB_simple.xlsx
+++ b/analysis/data/supplementary_data/sample_macroscopicTB_simple.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meran\Documents\Archaeology\PhD\Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meran\Documents\workflows\article1\analysis\data\supplementary_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD78B563-D0C4-4113-8B79-EB6373AF83AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857D249B-31AF-4E50-A18D-7CD74B1AB62D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BC839283-5A30-47EE-BE24-B4CF6A7F82B6}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="200">
   <si>
     <t>Jordana</t>
   </si>
@@ -605,6 +605,39 @@
   </si>
   <si>
     <t>Praia da Mareta</t>
+  </si>
+  <si>
+    <t>10YR 4/1, 10 YR 5/2, 10YR 6/2</t>
+  </si>
+  <si>
+    <t>5YR 6/2</t>
+  </si>
+  <si>
+    <t>10YR 6/1, 10YR 7/1, 10YR 8/1</t>
+  </si>
+  <si>
+    <t>2.5YR 6/1, 10R 4/3, 10R 8/2</t>
+  </si>
+  <si>
+    <t>10YR 5/2, 10YR 5/3</t>
+  </si>
+  <si>
+    <t>10YR 7/2, 10YR 6/2</t>
+  </si>
+  <si>
+    <t>10YR 8/2, 10YR 7/1</t>
+  </si>
+  <si>
+    <t>2.5Y 6/2, 2.5Y 7/4, 2.5Y 8/1, 5RP 6/2, 5RP 4/2</t>
+  </si>
+  <si>
+    <t>10YR 7/1, 10YR 8/1, 10YR 8/2</t>
+  </si>
+  <si>
+    <t>10YR 5/1, 10YR 6/1, 10YR 7/1</t>
+  </si>
+  <si>
+    <t>10YR 8/2, 10YR 6/3</t>
   </si>
 </sst>
 </file>
@@ -968,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A96E85-60C5-42AF-9B9A-F89D3153C625}">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1035,6 +1068,9 @@
       <c r="C2" t="s">
         <v>46</v>
       </c>
+      <c r="D2" t="s">
+        <v>191</v>
+      </c>
       <c r="E2" t="s">
         <v>15</v>
       </c>
@@ -1070,6 +1106,9 @@
       <c r="C3" t="s">
         <v>47</v>
       </c>
+      <c r="D3" t="s">
+        <v>192</v>
+      </c>
       <c r="E3" t="s">
         <v>15</v>
       </c>
@@ -1105,6 +1144,9 @@
       <c r="C4" t="s">
         <v>47</v>
       </c>
+      <c r="D4" t="s">
+        <v>191</v>
+      </c>
       <c r="E4" t="s">
         <v>15</v>
       </c>
@@ -1140,6 +1182,9 @@
       <c r="C5" t="s">
         <v>46</v>
       </c>
+      <c r="D5" t="s">
+        <v>191</v>
+      </c>
       <c r="E5" t="s">
         <v>15</v>
       </c>
@@ -1175,6 +1220,9 @@
       <c r="C6" t="s">
         <v>47</v>
       </c>
+      <c r="D6" t="s">
+        <v>189</v>
+      </c>
       <c r="E6" t="s">
         <v>15</v>
       </c>
@@ -1248,6 +1296,9 @@
       <c r="C8" t="s">
         <v>48</v>
       </c>
+      <c r="D8" t="s">
+        <v>190</v>
+      </c>
       <c r="E8" t="s">
         <v>15</v>
       </c>
@@ -1283,6 +1334,9 @@
       <c r="C9" t="s">
         <v>47</v>
       </c>
+      <c r="D9" t="s">
+        <v>196</v>
+      </c>
       <c r="E9" t="s">
         <v>15</v>
       </c>
@@ -1318,6 +1372,9 @@
       <c r="C10" t="s">
         <v>47</v>
       </c>
+      <c r="D10" t="s">
+        <v>197</v>
+      </c>
       <c r="E10" t="s">
         <v>15</v>
       </c>
@@ -1527,7 +1584,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -1537,6 +1594,9 @@
       <c r="C16" t="s">
         <v>47</v>
       </c>
+      <c r="D16" s="1" t="s">
+        <v>195</v>
+      </c>
       <c r="E16" t="s">
         <v>15</v>
       </c>
@@ -1562,7 +1622,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -1572,6 +1632,9 @@
       <c r="C17" t="s">
         <v>47</v>
       </c>
+      <c r="D17" s="1" t="s">
+        <v>199</v>
+      </c>
       <c r="E17" t="s">
         <v>15</v>
       </c>
@@ -1597,7 +1660,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -1606,6 +1669,9 @@
       </c>
       <c r="C18" t="s">
         <v>46</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="E18" t="s">
         <v>15</v>
@@ -1642,6 +1708,9 @@
       <c r="C19" t="s">
         <v>46</v>
       </c>
+      <c r="D19" t="s">
+        <v>193</v>
+      </c>
       <c r="E19" t="s">
         <v>15</v>
       </c>
@@ -1677,6 +1746,9 @@
       <c r="C20" t="s">
         <v>46</v>
       </c>
+      <c r="D20" t="s">
+        <v>193</v>
+      </c>
       <c r="E20" t="s">
         <v>15</v>
       </c>
@@ -1712,6 +1784,9 @@
       <c r="C21" t="s">
         <v>47</v>
       </c>
+      <c r="D21" t="s">
+        <v>198</v>
+      </c>
       <c r="E21" t="s">
         <v>15</v>
       </c>
@@ -2915,7 +2990,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" ht="15" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>170</v>
       </c>
@@ -2924,6 +2999,9 @@
       </c>
       <c r="C53" t="s">
         <v>48</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="E53" t="s">
         <v>15</v>

</xml_diff>